<commit_message>
May 9 update current day
</commit_message>
<xml_diff>
--- a/SSBBUe_Schedule.xlsx
+++ b/SSBBUe_Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\works\01_Project\03_SS_BBUe\01_Init\04_Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\works\04_Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07E3B0A-2B36-4A70-A25F-C982D91C82CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2893F4D-2BBD-47DD-9748-89D88CD1EE5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="793" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2448,54 +2448,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2517,6 +2469,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2525,6 +2492,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -8534,14 +8534,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -8558,7 +8558,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4810125" y="1162050"/>
+          <a:off x="5076825" y="1162050"/>
           <a:ext cx="0" cy="14658975"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -12876,15 +12876,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="36"/>
@@ -12894,11 +12894,11 @@
       <c r="F3" s="37"/>
     </row>
     <row r="4" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="40" t="s">
         <v>40</v>
       </c>
@@ -12913,13 +12913,13 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="66" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="43" t="s">
@@ -12934,9 +12934,9 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="80"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="74"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="67"/>
       <c r="E6" s="43" t="s">
         <v>22</v>
       </c>
@@ -12949,8 +12949,8 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="80"/>
-      <c r="C7" s="81"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="65"/>
       <c r="D7" s="42" t="s">
         <v>41</v>
       </c>
@@ -12966,17 +12966,17 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="80"/>
-      <c r="C8" s="81" t="s">
+      <c r="B8" s="64"/>
+      <c r="C8" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="82" t="s">
+      <c r="D8" s="71" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="68" t="s">
         <v>51</v>
       </c>
       <c r="G8" s="44"/>
@@ -12985,93 +12985,93 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="80"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="83"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="72"/>
       <c r="E9" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="66"/>
+      <c r="F9" s="70"/>
       <c r="G9" s="44"/>
       <c r="H9" s="45" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="80"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="83"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="66"/>
+      <c r="F10" s="70"/>
       <c r="G10" s="44"/>
       <c r="H10" s="45" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="80"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="83"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="72"/>
       <c r="E11" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="66"/>
+      <c r="F11" s="70"/>
       <c r="G11" s="44"/>
       <c r="H11" s="45" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B12" s="80"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="83"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="72"/>
       <c r="E12" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="66"/>
+      <c r="F12" s="70"/>
       <c r="G12" s="44"/>
       <c r="H12" s="42" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="80"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="83"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="66"/>
+      <c r="F13" s="70"/>
       <c r="G13" s="44"/>
       <c r="H13" s="42" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="80"/>
-      <c r="C14" s="81"/>
-      <c r="D14" s="84"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="73"/>
       <c r="E14" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="60"/>
+      <c r="F14" s="69"/>
       <c r="G14" s="44"/>
       <c r="H14" s="49" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="80"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="72" t="s">
+      <c r="B15" s="64"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="66" t="s">
         <v>58</v>
       </c>
       <c r="E15" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="59" t="s">
+      <c r="F15" s="68" t="s">
         <v>59</v>
       </c>
       <c r="G15" s="44"/>
@@ -13080,80 +13080,80 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="80"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="73"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="74"/>
       <c r="E16" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="66"/>
+      <c r="F16" s="70"/>
       <c r="G16" s="44"/>
       <c r="H16" s="42" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="80"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="73"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="74"/>
       <c r="E17" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="66"/>
+      <c r="F17" s="70"/>
       <c r="G17" s="44"/>
       <c r="H17" s="42" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="B18" s="80"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="73"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="74"/>
       <c r="E18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="66"/>
+      <c r="F18" s="70"/>
       <c r="G18" s="44"/>
       <c r="H18" s="42" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="80"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="73"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="74"/>
       <c r="E19" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="66"/>
+      <c r="F19" s="70"/>
       <c r="G19" s="44"/>
       <c r="H19" s="42" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="80"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="74"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="67"/>
       <c r="E20" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="60"/>
+      <c r="F20" s="69"/>
       <c r="G20" s="44"/>
       <c r="H20" s="42" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="80"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="72" t="s">
+      <c r="B21" s="64"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="66" t="s">
         <v>67</v>
       </c>
       <c r="E21" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="59" t="s">
+      <c r="F21" s="68" t="s">
         <v>68</v>
       </c>
       <c r="G21" s="44"/>
@@ -13162,28 +13162,28 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="80"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="74"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="67"/>
       <c r="E22" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="60"/>
+      <c r="F22" s="69"/>
       <c r="G22" s="44"/>
       <c r="H22" s="42" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="80"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="72" t="s">
+      <c r="B23" s="64"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="66" t="s">
         <v>71</v>
       </c>
       <c r="E23" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="59" t="s">
+      <c r="F23" s="68" t="s">
         <v>72</v>
       </c>
       <c r="G23" s="44"/>
@@ -13192,34 +13192,34 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="80"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="73"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="74"/>
       <c r="E24" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="66"/>
+      <c r="F24" s="70"/>
       <c r="G24" s="44"/>
       <c r="H24" s="42" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="80"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="74"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="67"/>
       <c r="E25" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="60"/>
+      <c r="F25" s="69"/>
       <c r="G25" s="44"/>
       <c r="H25" s="42" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="80"/>
-      <c r="C26" s="81"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="65"/>
       <c r="D26" s="42" t="s">
         <v>76</v>
       </c>
@@ -13235,8 +13235,8 @@
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="80"/>
-      <c r="C27" s="81"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="65"/>
       <c r="D27" s="42" t="s">
         <v>79</v>
       </c>
@@ -13252,8 +13252,8 @@
       </c>
     </row>
     <row r="28" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B28" s="80"/>
-      <c r="C28" s="81"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="65"/>
       <c r="D28" s="42" t="s">
         <v>82</v>
       </c>
@@ -13269,8 +13269,8 @@
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="80"/>
-      <c r="C29" s="81"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="65"/>
       <c r="D29" s="42" t="s">
         <v>93</v>
       </c>
@@ -13286,8 +13286,8 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="80"/>
-      <c r="C30" s="81"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="65"/>
       <c r="D30" s="42" t="s">
         <v>96</v>
       </c>
@@ -13303,8 +13303,8 @@
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="80"/>
-      <c r="C31" s="81"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="65"/>
       <c r="D31" s="42" t="s">
         <v>99</v>
       </c>
@@ -13320,8 +13320,8 @@
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="80"/>
-      <c r="C32" s="81" t="s">
+      <c r="B32" s="64"/>
+      <c r="C32" s="65" t="s">
         <v>85</v>
       </c>
       <c r="D32" s="45" t="s">
@@ -13339,15 +13339,15 @@
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="80"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="61" t="s">
+      <c r="B33" s="64"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="75" t="s">
         <v>89</v>
       </c>
       <c r="E33" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="59" t="s">
+      <c r="F33" s="68" t="s">
         <v>90</v>
       </c>
       <c r="G33" s="45"/>
@@ -13356,13 +13356,13 @@
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="80"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="62"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="76"/>
       <c r="E34" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="69"/>
       <c r="G34" s="45"/>
       <c r="H34" s="45" t="s">
         <v>92</v>
@@ -13370,15 +13370,15 @@
       <c r="I34" s="46"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="80"/>
-      <c r="C35" s="81"/>
-      <c r="D35" s="69" t="s">
+      <c r="B35" s="64"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="77" t="s">
         <v>102</v>
       </c>
       <c r="E35" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="59" t="s">
+      <c r="F35" s="68" t="s">
         <v>103</v>
       </c>
       <c r="G35" s="45"/>
@@ -13388,13 +13388,13 @@
       <c r="I35" s="46"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="80"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="70"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="78"/>
       <c r="E36" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F36" s="66"/>
+      <c r="F36" s="70"/>
       <c r="G36" s="45"/>
       <c r="H36" s="45" t="s">
         <v>52</v>
@@ -13402,13 +13402,13 @@
       <c r="I36" s="46"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="80"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="70"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="78"/>
       <c r="E37" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F37" s="66"/>
+      <c r="F37" s="70"/>
       <c r="G37" s="45"/>
       <c r="H37" s="45" t="s">
         <v>53</v>
@@ -13416,67 +13416,67 @@
       <c r="I37" s="46"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="80"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="70"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="78"/>
       <c r="E38" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F38" s="66"/>
+      <c r="F38" s="70"/>
       <c r="G38" s="45"/>
       <c r="H38" s="45" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="39" spans="2:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B39" s="80"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="70"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="78"/>
       <c r="E39" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F39" s="66"/>
+      <c r="F39" s="70"/>
       <c r="G39" s="45"/>
       <c r="H39" s="42" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="80"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="70"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="78"/>
       <c r="E40" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F40" s="66"/>
+      <c r="F40" s="70"/>
       <c r="G40" s="45"/>
       <c r="H40" s="42" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="80"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="71"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="79"/>
       <c r="E41" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="F41" s="60"/>
+      <c r="F41" s="69"/>
       <c r="G41" s="45"/>
       <c r="H41" s="49" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="42" spans="2:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="B42" s="80"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="61" t="s">
+      <c r="B42" s="64"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="75" t="s">
         <v>104</v>
       </c>
       <c r="E42" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F42" s="59" t="s">
+      <c r="F42" s="68" t="s">
         <v>105</v>
       </c>
       <c r="G42" s="45"/>
@@ -13485,41 +13485,41 @@
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="80"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="65"/>
+      <c r="B43" s="64"/>
+      <c r="C43" s="65"/>
+      <c r="D43" s="80"/>
       <c r="E43" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F43" s="66"/>
+      <c r="F43" s="70"/>
       <c r="G43" s="45"/>
       <c r="H43" s="45" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="80"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="62"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="76"/>
       <c r="E44" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F44" s="60"/>
+      <c r="F44" s="69"/>
       <c r="G44" s="45"/>
       <c r="H44" s="45" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="45" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B45" s="80"/>
-      <c r="C45" s="81"/>
-      <c r="D45" s="61" t="s">
+      <c r="B45" s="64"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="75" t="s">
         <v>108</v>
       </c>
       <c r="E45" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F45" s="59" t="s">
+      <c r="F45" s="68" t="s">
         <v>109</v>
       </c>
       <c r="G45" s="45"/>
@@ -13528,132 +13528,132 @@
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="80"/>
-      <c r="C46" s="81"/>
-      <c r="D46" s="65"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="80"/>
       <c r="E46" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="66"/>
+      <c r="F46" s="70"/>
       <c r="G46" s="45"/>
       <c r="H46" s="42" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B47" s="80"/>
-      <c r="C47" s="81"/>
-      <c r="D47" s="65"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="80"/>
       <c r="E47" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="66"/>
+      <c r="F47" s="70"/>
       <c r="G47" s="45"/>
       <c r="H47" s="42" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B48" s="80"/>
-      <c r="C48" s="81"/>
-      <c r="D48" s="65"/>
+      <c r="B48" s="64"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="80"/>
       <c r="E48" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="66"/>
+      <c r="F48" s="70"/>
       <c r="G48" s="45"/>
       <c r="H48" s="42" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="80"/>
-      <c r="C49" s="81"/>
-      <c r="D49" s="65"/>
+      <c r="B49" s="64"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="80"/>
       <c r="E49" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F49" s="66"/>
+      <c r="F49" s="70"/>
       <c r="G49" s="45"/>
       <c r="H49" s="42" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="50" spans="2:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="B50" s="80"/>
-      <c r="C50" s="81"/>
-      <c r="D50" s="65"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="65"/>
+      <c r="D50" s="80"/>
       <c r="E50" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F50" s="66"/>
+      <c r="F50" s="70"/>
       <c r="G50" s="45"/>
       <c r="H50" s="42" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B51" s="80"/>
-      <c r="C51" s="81"/>
-      <c r="D51" s="65"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="65"/>
+      <c r="D51" s="80"/>
       <c r="E51" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F51" s="66"/>
+      <c r="F51" s="70"/>
       <c r="G51" s="45"/>
       <c r="H51" s="42" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B52" s="80"/>
-      <c r="C52" s="81"/>
-      <c r="D52" s="65"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="80"/>
       <c r="E52" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="F52" s="66"/>
+      <c r="F52" s="70"/>
       <c r="G52" s="45"/>
       <c r="H52" s="42" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B53" s="80"/>
-      <c r="C53" s="81"/>
-      <c r="D53" s="65"/>
+      <c r="B53" s="64"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="80"/>
       <c r="E53" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F53" s="66"/>
+      <c r="F53" s="70"/>
       <c r="G53" s="45"/>
       <c r="H53" s="45" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B54" s="80"/>
-      <c r="C54" s="81"/>
-      <c r="D54" s="62"/>
+      <c r="B54" s="64"/>
+      <c r="C54" s="65"/>
+      <c r="D54" s="76"/>
       <c r="E54" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F54" s="60"/>
+      <c r="F54" s="69"/>
       <c r="G54" s="45"/>
       <c r="H54" s="45" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B55" s="80"/>
-      <c r="C55" s="81"/>
-      <c r="D55" s="67" t="s">
+      <c r="B55" s="64"/>
+      <c r="C55" s="65"/>
+      <c r="D55" s="81" t="s">
         <v>111</v>
       </c>
       <c r="E55" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F55" s="59" t="s">
+      <c r="F55" s="68" t="s">
         <v>114</v>
       </c>
       <c r="G55" s="45"/>
@@ -13662,28 +13662,28 @@
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B56" s="80"/>
-      <c r="C56" s="81"/>
-      <c r="D56" s="68"/>
+      <c r="B56" s="64"/>
+      <c r="C56" s="65"/>
+      <c r="D56" s="82"/>
       <c r="E56" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F56" s="60"/>
+      <c r="F56" s="69"/>
       <c r="G56" s="45"/>
       <c r="H56" s="45" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B57" s="80"/>
-      <c r="C57" s="81"/>
-      <c r="D57" s="61" t="s">
+      <c r="B57" s="64"/>
+      <c r="C57" s="65"/>
+      <c r="D57" s="75" t="s">
         <v>115</v>
       </c>
       <c r="E57" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F57" s="59" t="s">
+      <c r="F57" s="68" t="s">
         <v>116</v>
       </c>
       <c r="G57" s="45"/>
@@ -13692,67 +13692,67 @@
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B58" s="80"/>
-      <c r="C58" s="81"/>
-      <c r="D58" s="65"/>
+      <c r="B58" s="64"/>
+      <c r="C58" s="65"/>
+      <c r="D58" s="80"/>
       <c r="E58" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F58" s="66"/>
+      <c r="F58" s="70"/>
       <c r="G58" s="45"/>
       <c r="H58" s="42" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B59" s="80"/>
-      <c r="C59" s="81"/>
-      <c r="D59" s="65"/>
+      <c r="B59" s="64"/>
+      <c r="C59" s="65"/>
+      <c r="D59" s="80"/>
       <c r="E59" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F59" s="66"/>
+      <c r="F59" s="70"/>
       <c r="G59" s="45"/>
       <c r="H59" s="45" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B60" s="80"/>
-      <c r="C60" s="81"/>
-      <c r="D60" s="65"/>
+      <c r="B60" s="64"/>
+      <c r="C60" s="65"/>
+      <c r="D60" s="80"/>
       <c r="E60" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F60" s="66"/>
+      <c r="F60" s="70"/>
       <c r="G60" s="45"/>
       <c r="H60" s="45" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B61" s="80"/>
-      <c r="C61" s="81"/>
-      <c r="D61" s="62"/>
+      <c r="B61" s="64"/>
+      <c r="C61" s="65"/>
+      <c r="D61" s="76"/>
       <c r="E61" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F61" s="60"/>
+      <c r="F61" s="69"/>
       <c r="G61" s="45"/>
       <c r="H61" s="42" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B62" s="80"/>
-      <c r="C62" s="81"/>
-      <c r="D62" s="61" t="s">
+      <c r="B62" s="64"/>
+      <c r="C62" s="65"/>
+      <c r="D62" s="75" t="s">
         <v>119</v>
       </c>
       <c r="E62" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F62" s="59" t="s">
+      <c r="F62" s="68" t="s">
         <v>120</v>
       </c>
       <c r="G62" s="45"/>
@@ -13761,28 +13761,28 @@
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B63" s="80"/>
-      <c r="C63" s="81"/>
-      <c r="D63" s="62"/>
+      <c r="B63" s="64"/>
+      <c r="C63" s="65"/>
+      <c r="D63" s="76"/>
       <c r="E63" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F63" s="60"/>
+      <c r="F63" s="69"/>
       <c r="G63" s="45"/>
       <c r="H63" s="45" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B64" s="80"/>
-      <c r="C64" s="81"/>
-      <c r="D64" s="61" t="s">
+      <c r="B64" s="64"/>
+      <c r="C64" s="65"/>
+      <c r="D64" s="75" t="s">
         <v>123</v>
       </c>
       <c r="E64" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F64" s="59" t="s">
+      <c r="F64" s="68" t="s">
         <v>124</v>
       </c>
       <c r="G64" s="45"/>
@@ -13791,26 +13791,26 @@
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B65" s="80"/>
-      <c r="C65" s="81"/>
-      <c r="D65" s="62"/>
+      <c r="B65" s="64"/>
+      <c r="C65" s="65"/>
+      <c r="D65" s="76"/>
       <c r="E65" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F65" s="60"/>
+      <c r="F65" s="69"/>
       <c r="G65" s="45"/>
       <c r="H65" s="45" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B66" s="80"/>
-      <c r="C66" s="81"/>
-      <c r="D66" s="61" t="s">
+      <c r="B66" s="64"/>
+      <c r="C66" s="65"/>
+      <c r="D66" s="75" t="s">
         <v>125</v>
       </c>
       <c r="E66" s="43"/>
-      <c r="F66" s="59" t="s">
+      <c r="F66" s="68" t="s">
         <v>126</v>
       </c>
       <c r="G66" s="45"/>
@@ -13819,47 +13819,47 @@
       </c>
     </row>
     <row r="67" spans="2:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="B67" s="80"/>
-      <c r="C67" s="81"/>
-      <c r="D67" s="65"/>
+      <c r="B67" s="64"/>
+      <c r="C67" s="65"/>
+      <c r="D67" s="80"/>
       <c r="E67" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F67" s="66"/>
+      <c r="F67" s="70"/>
       <c r="G67" s="45"/>
       <c r="H67" s="42" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="68" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B68" s="80"/>
-      <c r="C68" s="81"/>
-      <c r="D68" s="65"/>
+      <c r="B68" s="64"/>
+      <c r="C68" s="65"/>
+      <c r="D68" s="80"/>
       <c r="E68" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F68" s="66"/>
+      <c r="F68" s="70"/>
       <c r="G68" s="45"/>
       <c r="H68" s="42" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B69" s="80"/>
-      <c r="C69" s="81"/>
-      <c r="D69" s="62"/>
+      <c r="B69" s="64"/>
+      <c r="C69" s="65"/>
+      <c r="D69" s="76"/>
       <c r="E69" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F69" s="60"/>
+      <c r="F69" s="69"/>
       <c r="G69" s="45"/>
       <c r="H69" s="45" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="70" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B70" s="80"/>
-      <c r="C70" s="81" t="s">
+      <c r="B70" s="64"/>
+      <c r="C70" s="65" t="s">
         <v>152</v>
       </c>
       <c r="D70" s="52" t="s">
@@ -13877,8 +13877,8 @@
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B71" s="80"/>
-      <c r="C71" s="81"/>
+      <c r="B71" s="64"/>
+      <c r="C71" s="65"/>
       <c r="D71" s="45" t="s">
         <v>143</v>
       </c>
@@ -13894,8 +13894,8 @@
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B72" s="80"/>
-      <c r="C72" s="81"/>
+      <c r="B72" s="64"/>
+      <c r="C72" s="65"/>
       <c r="D72" s="45" t="s">
         <v>146</v>
       </c>
@@ -13911,15 +13911,15 @@
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B73" s="80"/>
-      <c r="C73" s="81"/>
-      <c r="D73" s="61" t="s">
+      <c r="B73" s="64"/>
+      <c r="C73" s="65"/>
+      <c r="D73" s="75" t="s">
         <v>153</v>
       </c>
       <c r="E73" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F73" s="59" t="s">
+      <c r="F73" s="68" t="s">
         <v>154</v>
       </c>
       <c r="G73" s="45"/>
@@ -13928,28 +13928,28 @@
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B74" s="80"/>
-      <c r="C74" s="81"/>
-      <c r="D74" s="62"/>
+      <c r="B74" s="64"/>
+      <c r="C74" s="65"/>
+      <c r="D74" s="76"/>
       <c r="E74" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F74" s="60"/>
+      <c r="F74" s="69"/>
       <c r="G74" s="45"/>
       <c r="H74" s="45" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B75" s="80"/>
-      <c r="C75" s="81"/>
-      <c r="D75" s="61" t="s">
+      <c r="B75" s="64"/>
+      <c r="C75" s="65"/>
+      <c r="D75" s="75" t="s">
         <v>157</v>
       </c>
       <c r="E75" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F75" s="59" t="s">
+      <c r="F75" s="68" t="s">
         <v>158</v>
       </c>
       <c r="G75" s="45"/>
@@ -13958,34 +13958,34 @@
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B76" s="80"/>
-      <c r="C76" s="81"/>
-      <c r="D76" s="65"/>
+      <c r="B76" s="64"/>
+      <c r="C76" s="65"/>
+      <c r="D76" s="80"/>
       <c r="E76" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F76" s="66"/>
+      <c r="F76" s="70"/>
       <c r="G76" s="45"/>
       <c r="H76" s="45" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B77" s="80"/>
-      <c r="C77" s="81"/>
-      <c r="D77" s="62"/>
+      <c r="B77" s="64"/>
+      <c r="C77" s="65"/>
+      <c r="D77" s="76"/>
       <c r="E77" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F77" s="60"/>
+      <c r="F77" s="69"/>
       <c r="G77" s="45"/>
       <c r="H77" s="45" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B78" s="80"/>
-      <c r="C78" s="81"/>
+      <c r="B78" s="64"/>
+      <c r="C78" s="65"/>
       <c r="D78" s="51" t="s">
         <v>162</v>
       </c>
@@ -14001,8 +14001,8 @@
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B79" s="80"/>
-      <c r="C79" s="81"/>
+      <c r="B79" s="64"/>
+      <c r="C79" s="65"/>
       <c r="D79" s="51" t="s">
         <v>164</v>
       </c>
@@ -14018,15 +14018,15 @@
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B80" s="80"/>
-      <c r="C80" s="81"/>
+      <c r="B80" s="64"/>
+      <c r="C80" s="65"/>
       <c r="D80" s="51" t="s">
         <v>169</v>
       </c>
       <c r="E80" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F80" s="59" t="s">
+      <c r="F80" s="68" t="s">
         <v>174</v>
       </c>
       <c r="G80" s="45"/>
@@ -14035,34 +14035,34 @@
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B81" s="80"/>
-      <c r="C81" s="81"/>
+      <c r="B81" s="64"/>
+      <c r="C81" s="65"/>
       <c r="D81" s="51"/>
       <c r="E81" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F81" s="66"/>
+      <c r="F81" s="70"/>
       <c r="G81" s="45"/>
       <c r="H81" s="45" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B82" s="80"/>
-      <c r="C82" s="81"/>
+      <c r="B82" s="64"/>
+      <c r="C82" s="65"/>
       <c r="D82" s="51"/>
       <c r="E82" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F82" s="60"/>
+      <c r="F82" s="69"/>
       <c r="G82" s="45"/>
       <c r="H82" s="45" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B83" s="80"/>
-      <c r="C83" s="81"/>
+      <c r="B83" s="64"/>
+      <c r="C83" s="65"/>
       <c r="D83" s="51" t="s">
         <v>173</v>
       </c>
@@ -14078,17 +14078,17 @@
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B84" s="80"/>
-      <c r="C84" s="63" t="s">
+      <c r="B84" s="64"/>
+      <c r="C84" s="83" t="s">
         <v>140</v>
       </c>
-      <c r="D84" s="61" t="s">
+      <c r="D84" s="75" t="s">
         <v>134</v>
       </c>
       <c r="E84" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F84" s="59" t="s">
+      <c r="F84" s="68" t="s">
         <v>135</v>
       </c>
       <c r="G84" s="45"/>
@@ -14097,28 +14097,28 @@
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B85" s="80"/>
-      <c r="C85" s="64"/>
-      <c r="D85" s="62"/>
+      <c r="B85" s="64"/>
+      <c r="C85" s="84"/>
+      <c r="D85" s="76"/>
       <c r="E85" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F85" s="60"/>
+      <c r="F85" s="69"/>
       <c r="G85" s="45"/>
       <c r="H85" s="45" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B86" s="80"/>
-      <c r="C86" s="64"/>
-      <c r="D86" s="61" t="s">
+      <c r="B86" s="64"/>
+      <c r="C86" s="84"/>
+      <c r="D86" s="75" t="s">
         <v>138</v>
       </c>
       <c r="E86" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F86" s="59" t="s">
+      <c r="F86" s="68" t="s">
         <v>139</v>
       </c>
       <c r="G86" s="45"/>
@@ -14127,21 +14127,21 @@
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B87" s="80"/>
-      <c r="C87" s="64"/>
-      <c r="D87" s="62"/>
+      <c r="B87" s="64"/>
+      <c r="C87" s="84"/>
+      <c r="D87" s="76"/>
       <c r="E87" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F87" s="60"/>
+      <c r="F87" s="69"/>
       <c r="G87" s="45"/>
       <c r="H87" s="45" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B88" s="80"/>
-      <c r="C88" s="64"/>
+      <c r="B88" s="64"/>
+      <c r="C88" s="84"/>
       <c r="D88" s="45" t="s">
         <v>141</v>
       </c>
@@ -14155,8 +14155,8 @@
       <c r="H88" s="45"/>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B89" s="80"/>
-      <c r="C89" s="64"/>
+      <c r="B89" s="64"/>
+      <c r="C89" s="84"/>
       <c r="D89" s="45" t="s">
         <v>166</v>
       </c>
@@ -14172,8 +14172,8 @@
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B90" s="80"/>
-      <c r="C90" s="64"/>
+      <c r="B90" s="64"/>
+      <c r="C90" s="84"/>
       <c r="D90" s="45" t="s">
         <v>176</v>
       </c>
@@ -14189,7 +14189,7 @@
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B91" s="80"/>
+      <c r="B91" s="64"/>
       <c r="C91" s="50" t="s">
         <v>178</v>
       </c>
@@ -14208,7 +14208,7 @@
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B92" s="80" t="s">
+      <c r="B92" s="64" t="s">
         <v>23</v>
       </c>
       <c r="C92" s="44" t="s">
@@ -14223,7 +14223,7 @@
       <c r="H92" s="45"/>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B93" s="80"/>
+      <c r="B93" s="64"/>
       <c r="C93" s="44" t="s">
         <v>25</v>
       </c>
@@ -14236,7 +14236,7 @@
       <c r="H93" s="45"/>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B94" s="80"/>
+      <c r="B94" s="64"/>
       <c r="C94" s="44" t="s">
         <v>0</v>
       </c>
@@ -14249,7 +14249,7 @@
       <c r="H94" s="45"/>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B95" s="80"/>
+      <c r="B95" s="64"/>
       <c r="C95" s="44" t="s">
         <v>1</v>
       </c>
@@ -14262,7 +14262,7 @@
       <c r="H95" s="45"/>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B96" s="80"/>
+      <c r="B96" s="64"/>
       <c r="C96" s="44" t="s">
         <v>2</v>
       </c>
@@ -14275,7 +14275,7 @@
       <c r="H96" s="45"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B97" s="80" t="s">
+      <c r="B97" s="64" t="s">
         <v>26</v>
       </c>
       <c r="C97" s="41" t="s">
@@ -14290,7 +14290,7 @@
       <c r="H97" s="45"/>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B98" s="80"/>
+      <c r="B98" s="64"/>
       <c r="C98" s="41" t="s">
         <v>28</v>
       </c>
@@ -14303,7 +14303,7 @@
       <c r="H98" s="45"/>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B99" s="80"/>
+      <c r="B99" s="64"/>
       <c r="C99" s="44" t="s">
         <v>29</v>
       </c>
@@ -14316,7 +14316,7 @@
       <c r="H99" s="45"/>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B100" s="80" t="s">
+      <c r="B100" s="64" t="s">
         <v>30</v>
       </c>
       <c r="C100" s="41" t="s">
@@ -14333,7 +14333,7 @@
       <c r="H100" s="45"/>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B101" s="80"/>
+      <c r="B101" s="64"/>
       <c r="C101" s="41" t="s">
         <v>33</v>
       </c>
@@ -14348,7 +14348,7 @@
       <c r="H101" s="45"/>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B102" s="80"/>
+      <c r="B102" s="64"/>
       <c r="C102" s="44" t="s">
         <v>35</v>
       </c>
@@ -14374,7 +14374,7 @@
       <c r="H103" s="45"/>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B104" s="75" t="s">
+      <c r="B104" s="59" t="s">
         <v>180</v>
       </c>
       <c r="C104" s="45" t="s">
@@ -14387,7 +14387,7 @@
       <c r="H104" s="45"/>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B105" s="76"/>
+      <c r="B105" s="60"/>
       <c r="C105" s="45" t="s">
         <v>182</v>
       </c>
@@ -14398,7 +14398,7 @@
       <c r="H105" s="45"/>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B106" s="77"/>
+      <c r="B106" s="61"/>
       <c r="C106" s="45" t="s">
         <v>237</v>
       </c>
@@ -14410,6 +14410,38 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="C84:C90"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="D75:D77"/>
+    <mergeCell ref="F75:F77"/>
+    <mergeCell ref="F80:F82"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="F66:F69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="F84:F85"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="D57:D61"/>
+    <mergeCell ref="F57:F61"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="F35:F41"/>
+    <mergeCell ref="D35:D41"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="D45:D54"/>
+    <mergeCell ref="F45:F54"/>
+    <mergeCell ref="D15:D20"/>
+    <mergeCell ref="F15:F20"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="D33:D34"/>
     <mergeCell ref="B104:B106"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B4:D4"/>
@@ -14426,38 +14458,6 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="F8:F14"/>
     <mergeCell ref="D8:D14"/>
-    <mergeCell ref="D15:D20"/>
-    <mergeCell ref="F15:F20"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="F35:F41"/>
-    <mergeCell ref="D35:D41"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="D45:D54"/>
-    <mergeCell ref="F45:F54"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="D57:D61"/>
-    <mergeCell ref="F57:F61"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="F84:F85"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="C84:C90"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="D75:D77"/>
-    <mergeCell ref="F75:F77"/>
-    <mergeCell ref="F80:F82"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>